<commit_message>
added info new drugs
</commit_message>
<xml_diff>
--- a/Data/CovidBox_Map.xlsx
+++ b/Data/CovidBox_Map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data_Drug_Screening_CovidBox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aernst\Documents\GitHub\CoVasc_DataApp\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="1600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="1604">
   <si>
     <t>STRUCTURE</t>
   </si>
@@ -16446,6 +16446,18 @@
   </si>
   <si>
     <t>https://www.thelancet.com/journals/laninf/article/PIIS1473-3099(16)30378-4/fulltext</t>
+  </si>
+  <si>
+    <t>Molnupiravir</t>
+  </si>
+  <si>
+    <t>Sabizabulin</t>
+  </si>
+  <si>
+    <t>Anti-infective agent - Cytoskeletal modulator</t>
+  </si>
+  <si>
+    <t>Addition</t>
   </si>
 </sst>
 </file>
@@ -24894,10 +24906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM161"/>
+  <dimension ref="A1:AM163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="N161" sqref="N161:N163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42206,6 +42218,46 @@
         <v>1599</v>
       </c>
     </row>
+    <row r="162" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+      <c r="C162" s="2" t="s">
+        <v>1600</v>
+      </c>
+      <c r="L162" s="2">
+        <v>3</v>
+      </c>
+      <c r="M162" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N162" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O162" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="V162" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="163" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+      <c r="C163" s="2" t="s">
+        <v>1601</v>
+      </c>
+      <c r="L163" s="2">
+        <v>3</v>
+      </c>
+      <c r="M163" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="N163" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O163" s="2" t="s">
+        <v>1602</v>
+      </c>
+      <c r="V163" t="s">
+        <v>1603</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="AA1:AA1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>